<commit_message>
180116 sangwoo schedule commit
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -284,7 +284,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -343,6 +343,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -715,7 +718,7 @@
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="15"/>
+      <c r="E5" s="20"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="10" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
180119 sangwoo schedule commit
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -736,8 +736,8 @@
       <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="20"/>
       <c r="P7" s="11"/>
       <c r="Q7" s="12"/>
       <c r="R7" s="13"/>

</xml_diff>